<commit_message>
207; integrate xls with DataProvider
</commit_message>
<xml_diff>
--- a/JaysTestFramework/SeleniumTestFramework/src/main/resources/seleniumTestData.xlsx
+++ b/JaysTestFramework/SeleniumTestFramework/src/main/resources/seleniumTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jay\training\repo\git\ud-selenium-B2A\JaysTestFramework\SeleniumTestFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02C0929-84E1-4F5D-B144-0E2AB2FAE71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A77EA1-9A8E-4D93-AB7F-81064C33E501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61365" yWindow="16575" windowWidth="19485" windowHeight="13770" xr2:uid="{2C69ABD7-6463-41B7-AE75-762E36EC4EC5}"/>
+    <workbookView xWindow="63285" yWindow="15720" windowWidth="19485" windowHeight="13770" activeTab="1" xr2:uid="{2C69ABD7-6463-41B7-AE75-762E36EC4EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>testcases</t>
   </si>
@@ -87,13 +87,37 @@
   </si>
   <si>
     <t>deleteprofiled3</t>
+  </si>
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>prodname</t>
+  </si>
+  <si>
+    <t>anshika@gmail.com</t>
+  </si>
+  <si>
+    <t>Iamking@000</t>
+  </si>
+  <si>
+    <t>ADIDAS ORIGINAL</t>
+  </si>
+  <si>
+    <t>ZARA COAT 3</t>
+  </si>
+  <si>
+    <t>IPHONE 13 PRO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +130,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2AA198"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,8 +158,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF85E410-611E-49EA-99FD-A37D43CEAD51}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,12 +564,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{579D995E-92DF-4081-B90D-C479320A91FD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="4" width="14.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>